<commit_message>
new errors are mentioned in the test file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Module</t>
   </si>
@@ -87,6 +87,45 @@
   </si>
   <si>
     <t>Transfer click krama add qualification enwa ,change reason wada ,acorian eka load wenawa</t>
+  </si>
+  <si>
+    <t>new errors -23/2/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Punishment </t>
+  </si>
+  <si>
+    <t>institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no place in the nav bar to add new punishments </t>
+  </si>
+  <si>
+    <t>no place in the nav bar to add new punishments</t>
+  </si>
+  <si>
+    <t>employee institute</t>
+  </si>
+  <si>
+    <t>heading wrong</t>
+  </si>
+  <si>
+    <t>nav bar error</t>
+  </si>
+  <si>
+    <t>button and singlish typing doent appear in the ui</t>
+  </si>
+  <si>
+    <t>cant chanage the color of the hour count box background color</t>
+  </si>
+  <si>
+    <t>drop down items arent visisble</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>acordian eke data visible nea</t>
   </si>
 </sst>
 </file>
@@ -124,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -147,11 +186,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -160,6 +210,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,16 +491,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G10"/>
+  <dimension ref="A2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
@@ -590,6 +641,66 @@
       </c>
       <c r="G10" s="1"/>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>